<commit_message>
sistemato 0 per datetime
</commit_message>
<xml_diff>
--- a/transm/flusso_modifica_parametro.xlsx
+++ b/transm/flusso_modifica_parametro.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giacomo.solazzi\Documents\sviluppo\src\arduino\a01\transm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A6CC3E-2296-4E9A-B0BA-9F944927EED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF2B438-A42B-47CF-81C6-3465519F24E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{50B162F0-49E0-43FE-8DCC-E6BD8AF511FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{50B162F0-49E0-43FE-8DCC-E6BD8AF511FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="codifica_stringhe" sheetId="2" r:id="rId2"/>
+    <sheet name="flusso" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">codifica_stringhe!$A$14:$J$31</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
   <si>
     <t>nexus 5</t>
   </si>
@@ -311,6 +312,18 @@
   </si>
   <si>
     <t>lunghezza totale caratteri</t>
+  </si>
+  <si>
+    <t>S070000000000300</t>
+  </si>
+  <si>
+    <t>stringa codificata x aggiornamento num skip, es imposta 3 skip = S070000000000300</t>
+  </si>
+  <si>
+    <t>ricordarsi di cambiare il nome delle variabili su arduino ev controller con il nome del parametro. Es numero skip S07 la corrispondente variabile è V07. Cambia solo la prima lettera che è sempre V</t>
+  </si>
+  <si>
+    <t>step</t>
   </si>
 </sst>
 </file>
@@ -373,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -382,9 +395,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -392,6 +402,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758455FE-FD8E-4BEF-BAF9-4D59972DAA34}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,14 +902,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1028,7 +1044,7 @@
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>89</v>
       </c>
       <c r="B10" s="2"/>
@@ -1037,41 +1053,44 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="2"/>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1550,4 +1569,176 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C80BEB-B1ED-43CF-8DDA-1DFBE9712527}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>